<commit_message>
Fix sale quantity prediction
Amend result into integral value
</commit_message>
<xml_diff>
--- a/data-mining/models/SaleQuantityPrediction.xlsx
+++ b/data-mining/models/SaleQuantityPrediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my-git\data-mining\DataMining\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D171CE47-97C3-4C67-AB2F-62286B5EC465}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A37F78E7-4760-4238-B21E-BF606FA926CB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{08E12DA9-D18C-4F22-97F5-EEEDD5A8F89B}"/>
   </bookViews>
@@ -388,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05778BF-5A00-4167-B7B3-82BB6A24E23C}">
   <dimension ref="A1:C2515"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2490" workbookViewId="0">
-      <selection activeCell="I2503" sqref="I2503"/>
+    <sheetView tabSelected="1" topLeftCell="A2219" workbookViewId="0">
+      <selection activeCell="C2241" sqref="C2241:C2515"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25043,7 +25043,7 @@
         <v>42826</v>
       </c>
       <c r="C2241">
-        <v>736.04333333333295</v>
+        <v>736</v>
       </c>
     </row>
     <row r="2242" spans="1:3" x14ac:dyDescent="0.25">
@@ -25051,7 +25051,7 @@
         <v>42827</v>
       </c>
       <c r="C2242">
-        <v>709.47166666666601</v>
+        <v>709</v>
       </c>
     </row>
     <row r="2243" spans="1:3" x14ac:dyDescent="0.25">
@@ -25059,7 +25059,7 @@
         <v>42828</v>
       </c>
       <c r="C2243">
-        <v>696.92166666666606</v>
+        <v>696</v>
       </c>
     </row>
     <row r="2244" spans="1:3" x14ac:dyDescent="0.25">
@@ -25067,7 +25067,7 @@
         <v>42829</v>
       </c>
       <c r="C2244">
-        <v>703.02166666666596</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2245" spans="1:3" x14ac:dyDescent="0.25">
@@ -25075,7 +25075,7 @@
         <v>42830</v>
       </c>
       <c r="C2245">
-        <v>705.32166666666603</v>
+        <v>705</v>
       </c>
     </row>
     <row r="2246" spans="1:3" x14ac:dyDescent="0.25">
@@ -25083,7 +25083,7 @@
         <v>42831</v>
       </c>
       <c r="C2246">
-        <v>703.37166666666599</v>
+        <v>703</v>
       </c>
     </row>
     <row r="2247" spans="1:3" x14ac:dyDescent="0.25">
@@ -25091,7 +25091,7 @@
         <v>42832</v>
       </c>
       <c r="C2247">
-        <v>721.29333333333295</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2248" spans="1:3" x14ac:dyDescent="0.25">
@@ -25099,7 +25099,7 @@
         <v>42833</v>
       </c>
       <c r="C2248">
-        <v>737.62333333333299</v>
+        <v>737</v>
       </c>
     </row>
     <row r="2249" spans="1:3" x14ac:dyDescent="0.25">
@@ -25107,7 +25107,7 @@
         <v>42834</v>
       </c>
       <c r="C2249">
-        <v>714.08277777777698</v>
+        <v>714</v>
       </c>
     </row>
     <row r="2250" spans="1:3" x14ac:dyDescent="0.25">
@@ -25115,7 +25115,7 @@
         <v>42835</v>
       </c>
       <c r="C2250">
-        <v>696.27277777777704</v>
+        <v>696</v>
       </c>
     </row>
     <row r="2251" spans="1:3" x14ac:dyDescent="0.25">
@@ -25123,7 +25123,7 @@
         <v>42836</v>
       </c>
       <c r="C2251">
-        <v>692.85877777777705</v>
+        <v>692</v>
       </c>
     </row>
     <row r="2252" spans="1:3" x14ac:dyDescent="0.25">
@@ -25131,7 +25131,7 @@
         <v>42837</v>
       </c>
       <c r="C2252">
-        <v>676.30433333333303</v>
+        <v>676</v>
       </c>
     </row>
     <row r="2253" spans="1:3" x14ac:dyDescent="0.25">
@@ -25139,7 +25139,7 @@
         <v>42838</v>
       </c>
       <c r="C2253">
-        <v>678.25766666666595</v>
+        <v>678</v>
       </c>
     </row>
     <row r="2254" spans="1:3" x14ac:dyDescent="0.25">
@@ -25147,7 +25147,7 @@
         <v>42839</v>
       </c>
       <c r="C2254">
-        <v>702.88366666666604</v>
+        <v>702</v>
       </c>
     </row>
     <row r="2255" spans="1:3" x14ac:dyDescent="0.25">
@@ -25155,7 +25155,7 @@
         <v>42840</v>
       </c>
       <c r="C2255">
-        <v>724.969333333333</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2256" spans="1:3" x14ac:dyDescent="0.25">
@@ -25163,7 +25163,7 @@
         <v>42841</v>
       </c>
       <c r="C2256">
-        <v>690.66166666666595</v>
+        <v>690</v>
       </c>
     </row>
     <row r="2257" spans="1:3" x14ac:dyDescent="0.25">
@@ -25171,7 +25171,7 @@
         <v>42842</v>
       </c>
       <c r="C2257">
-        <v>291.06608333333298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2258" spans="1:3" x14ac:dyDescent="0.25">
@@ -25179,7 +25179,7 @@
         <v>42843</v>
       </c>
       <c r="C2258">
-        <v>291.89924999999999</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2259" spans="1:3" x14ac:dyDescent="0.25">
@@ -25187,7 +25187,7 @@
         <v>42844</v>
       </c>
       <c r="C2259">
-        <v>291.18539285714201</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2260" spans="1:3" x14ac:dyDescent="0.25">
@@ -25195,7 +25195,7 @@
         <v>42845</v>
       </c>
       <c r="C2260">
-        <v>288.15472619047603</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2261" spans="1:3" x14ac:dyDescent="0.25">
@@ -25203,7 +25203,7 @@
         <v>42846</v>
       </c>
       <c r="C2261">
-        <v>316.56683333333302</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2262" spans="1:3" x14ac:dyDescent="0.25">
@@ -25211,7 +25211,7 @@
         <v>42847</v>
       </c>
       <c r="C2262">
-        <v>377.26249999999999</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2263" spans="1:3" x14ac:dyDescent="0.25">
@@ -25219,7 +25219,7 @@
         <v>42848</v>
       </c>
       <c r="C2263">
-        <v>352.89666666666602</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2264" spans="1:3" x14ac:dyDescent="0.25">
@@ -25227,7 +25227,7 @@
         <v>42849</v>
       </c>
       <c r="C2264">
-        <v>308.87158333333298</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2265" spans="1:3" x14ac:dyDescent="0.25">
@@ -25235,7 +25235,7 @@
         <v>42850</v>
       </c>
       <c r="C2265">
-        <v>308.79291666666597</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2266" spans="1:3" x14ac:dyDescent="0.25">
@@ -25243,7 +25243,7 @@
         <v>42851</v>
       </c>
       <c r="C2266">
-        <v>306.67241666666598</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2267" spans="1:3" x14ac:dyDescent="0.25">
@@ -25251,7 +25251,7 @@
         <v>42852</v>
       </c>
       <c r="C2267">
-        <v>312.837416666666</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2268" spans="1:3" x14ac:dyDescent="0.25">
@@ -25259,7 +25259,7 @@
         <v>42853</v>
       </c>
       <c r="C2268">
-        <v>329.34583333333302</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2269" spans="1:3" x14ac:dyDescent="0.25">
@@ -25267,7 +25267,7 @@
         <v>42854</v>
       </c>
       <c r="C2269">
-        <v>376.11</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2270" spans="1:3" x14ac:dyDescent="0.25">
@@ -25275,7 +25275,7 @@
         <v>42855</v>
       </c>
       <c r="C2270">
-        <v>342.76666666666603</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2271" spans="1:3" x14ac:dyDescent="0.25">
@@ -25283,7 +25283,7 @@
         <v>42856</v>
       </c>
       <c r="C2271">
-        <v>276.48469047619</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2272" spans="1:3" x14ac:dyDescent="0.25">
@@ -25291,7 +25291,7 @@
         <v>42857</v>
       </c>
       <c r="C2272">
-        <v>275.47635714285701</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2273" spans="1:3" x14ac:dyDescent="0.25">
@@ -25299,7 +25299,7 @@
         <v>42858</v>
       </c>
       <c r="C2273">
-        <v>277.36594047619002</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2274" spans="1:3" x14ac:dyDescent="0.25">
@@ -25307,7 +25307,7 @@
         <v>42859</v>
       </c>
       <c r="C2274">
-        <v>287.04294047618998</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2275" spans="1:3" x14ac:dyDescent="0.25">
@@ -25315,7 +25315,7 @@
         <v>42860</v>
       </c>
       <c r="C2275">
-        <v>315.56083333333299</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2276" spans="1:3" x14ac:dyDescent="0.25">
@@ -25323,7 +25323,7 @@
         <v>42861</v>
       </c>
       <c r="C2276">
-        <v>373.24416666666599</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2277" spans="1:3" x14ac:dyDescent="0.25">
@@ -25331,7 +25331,7 @@
         <v>42862</v>
       </c>
       <c r="C2277">
-        <v>320.35750000000002</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2278" spans="1:3" x14ac:dyDescent="0.25">
@@ -25339,7 +25339,7 @@
         <v>42863</v>
       </c>
       <c r="C2278">
-        <v>282.66710714285699</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2279" spans="1:3" x14ac:dyDescent="0.25">
@@ -25347,7 +25347,7 @@
         <v>42864</v>
       </c>
       <c r="C2279">
-        <v>281.53877380952298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2280" spans="1:3" x14ac:dyDescent="0.25">
@@ -25355,7 +25355,7 @@
         <v>42865</v>
       </c>
       <c r="C2280">
-        <v>280.91710714285699</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2281" spans="1:3" x14ac:dyDescent="0.25">
@@ -25363,7 +25363,7 @@
         <v>42866</v>
       </c>
       <c r="C2281">
-        <v>283.62210714285698</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2282" spans="1:3" x14ac:dyDescent="0.25">
@@ -25371,7 +25371,7 @@
         <v>42867</v>
       </c>
       <c r="C2282">
-        <v>310.02749999999997</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2283" spans="1:3" x14ac:dyDescent="0.25">
@@ -25379,7 +25379,7 @@
         <v>42868</v>
       </c>
       <c r="C2283">
-        <v>363.24416666666599</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2284" spans="1:3" x14ac:dyDescent="0.25">
@@ -25387,7 +25387,7 @@
         <v>42869</v>
       </c>
       <c r="C2284">
-        <v>318.14583333333297</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2285" spans="1:3" x14ac:dyDescent="0.25">
@@ -25395,7 +25395,7 @@
         <v>42870</v>
       </c>
       <c r="C2285">
-        <v>282.39641666666603</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2286" spans="1:3" x14ac:dyDescent="0.25">
@@ -25403,7 +25403,7 @@
         <v>42871</v>
       </c>
       <c r="C2286">
-        <v>279.81708333333302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2287" spans="1:3" x14ac:dyDescent="0.25">
@@ -25411,7 +25411,7 @@
         <v>42872</v>
       </c>
       <c r="C2287">
-        <v>277.98874999999998</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2288" spans="1:3" x14ac:dyDescent="0.25">
@@ -25419,7 +25419,7 @@
         <v>42873</v>
       </c>
       <c r="C2288">
-        <v>276.73941666666599</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2289" spans="1:3" x14ac:dyDescent="0.25">
@@ -25427,7 +25427,7 @@
         <v>42874</v>
       </c>
       <c r="C2289">
-        <v>300.04583333333301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2290" spans="1:3" x14ac:dyDescent="0.25">
@@ -25435,7 +25435,7 @@
         <v>42875</v>
       </c>
       <c r="C2290">
-        <v>336.60750000000002</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2291" spans="1:3" x14ac:dyDescent="0.25">
@@ -25443,7 +25443,7 @@
         <v>42876</v>
       </c>
       <c r="C2291">
-        <v>313.264833333333</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2292" spans="1:3" x14ac:dyDescent="0.25">
@@ -25451,7 +25451,7 @@
         <v>42877</v>
       </c>
       <c r="C2292">
-        <v>283.47908333333299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2293" spans="1:3" x14ac:dyDescent="0.25">
@@ -25459,7 +25459,7 @@
         <v>42878</v>
       </c>
       <c r="C2293">
-        <v>294.79258333333303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2294" spans="1:3" x14ac:dyDescent="0.25">
@@ -25467,7 +25467,7 @@
         <v>42879</v>
       </c>
       <c r="C2294">
-        <v>289.34924999999998</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2295" spans="1:3" x14ac:dyDescent="0.25">
@@ -25475,7 +25475,7 @@
         <v>42880</v>
       </c>
       <c r="C2295">
-        <v>297.731916666666</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2296" spans="1:3" x14ac:dyDescent="0.25">
@@ -25483,7 +25483,7 @@
         <v>42881</v>
       </c>
       <c r="C2296">
-        <v>312.674166666666</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2297" spans="1:3" x14ac:dyDescent="0.25">
@@ -25491,7 +25491,7 @@
         <v>42882</v>
       </c>
       <c r="C2297">
-        <v>345.37166666666599</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2298" spans="1:3" x14ac:dyDescent="0.25">
@@ -25499,7 +25499,7 @@
         <v>42883</v>
       </c>
       <c r="C2298">
-        <v>320.93150000000003</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2299" spans="1:3" x14ac:dyDescent="0.25">
@@ -25507,7 +25507,7 @@
         <v>42884</v>
       </c>
       <c r="C2299">
-        <v>295.41174999999998</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2300" spans="1:3" x14ac:dyDescent="0.25">
@@ -25515,7 +25515,7 @@
         <v>42885</v>
       </c>
       <c r="C2300">
-        <v>291.10341666666602</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2301" spans="1:3" x14ac:dyDescent="0.25">
@@ -25523,7 +25523,7 @@
         <v>42886</v>
       </c>
       <c r="C2301">
-        <v>288.65758333333298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2302" spans="1:3" x14ac:dyDescent="0.25">
@@ -25531,7 +25531,7 @@
         <v>42887</v>
       </c>
       <c r="C2302">
-        <v>278.82135714285698</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2303" spans="1:3" x14ac:dyDescent="0.25">
@@ -25539,7 +25539,7 @@
         <v>42888</v>
       </c>
       <c r="C2303">
-        <v>305.87133333333298</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2304" spans="1:3" x14ac:dyDescent="0.25">
@@ -25547,7 +25547,7 @@
         <v>42889</v>
       </c>
       <c r="C2304">
-        <v>371.56666666666598</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2305" spans="1:3" x14ac:dyDescent="0.25">
@@ -25555,7 +25555,7 @@
         <v>42890</v>
       </c>
       <c r="C2305">
-        <v>320.76833333333298</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2306" spans="1:3" x14ac:dyDescent="0.25">
@@ -25563,7 +25563,7 @@
         <v>42891</v>
       </c>
       <c r="C2306">
-        <v>285.037107142857</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2307" spans="1:3" x14ac:dyDescent="0.25">
@@ -25571,7 +25571,7 @@
         <v>42892</v>
       </c>
       <c r="C2307">
-        <v>281.80377380952302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2308" spans="1:3" x14ac:dyDescent="0.25">
@@ -25579,7 +25579,7 @@
         <v>42893</v>
       </c>
       <c r="C2308">
-        <v>280.66544047618999</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2309" spans="1:3" x14ac:dyDescent="0.25">
@@ -25587,7 +25587,7 @@
         <v>42894</v>
       </c>
       <c r="C2309">
-        <v>283.43044047618997</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2310" spans="1:3" x14ac:dyDescent="0.25">
@@ -25595,7 +25595,7 @@
         <v>42895</v>
       </c>
       <c r="C2310">
-        <v>310.64083333333298</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2311" spans="1:3" x14ac:dyDescent="0.25">
@@ -25603,7 +25603,7 @@
         <v>42896</v>
       </c>
       <c r="C2311">
-        <v>370.57416666666597</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2312" spans="1:3" x14ac:dyDescent="0.25">
@@ -25611,7 +25611,7 @@
         <v>42897</v>
       </c>
       <c r="C2312">
-        <v>321.13083333333299</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2313" spans="1:3" x14ac:dyDescent="0.25">
@@ -25619,7 +25619,7 @@
         <v>42898</v>
       </c>
       <c r="C2313">
-        <v>284.02158333333301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2314" spans="1:3" x14ac:dyDescent="0.25">
@@ -25627,7 +25627,7 @@
         <v>42899</v>
       </c>
       <c r="C2314">
-        <v>282.34224999999901</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2315" spans="1:3" x14ac:dyDescent="0.25">
@@ -25635,7 +25635,7 @@
         <v>42900</v>
       </c>
       <c r="C2315">
-        <v>279.66141666666601</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2316" spans="1:3" x14ac:dyDescent="0.25">
@@ -25643,7 +25643,7 @@
         <v>42901</v>
       </c>
       <c r="C2316">
-        <v>278.919749999999</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2317" spans="1:3" x14ac:dyDescent="0.25">
@@ -25651,7 +25651,7 @@
         <v>42902</v>
       </c>
       <c r="C2317">
-        <v>302.23583333333301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2318" spans="1:3" x14ac:dyDescent="0.25">
@@ -25659,7 +25659,7 @@
         <v>42903</v>
       </c>
       <c r="C2318">
-        <v>343.64416666666602</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2319" spans="1:3" x14ac:dyDescent="0.25">
@@ -25667,7 +25667,7 @@
         <v>42904</v>
       </c>
       <c r="C2319">
-        <v>316.74983333333302</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2320" spans="1:3" x14ac:dyDescent="0.25">
@@ -25675,7 +25675,7 @@
         <v>42905</v>
       </c>
       <c r="C2320">
-        <v>282.11775</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2321" spans="1:3" x14ac:dyDescent="0.25">
@@ -25683,7 +25683,7 @@
         <v>42906</v>
       </c>
       <c r="C2321">
-        <v>276.99108333333299</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2322" spans="1:3" x14ac:dyDescent="0.25">
@@ -25691,7 +25691,7 @@
         <v>42907</v>
       </c>
       <c r="C2322">
-        <v>273.277749999999</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2323" spans="1:3" x14ac:dyDescent="0.25">
@@ -25699,7 +25699,7 @@
         <v>42908</v>
       </c>
       <c r="C2323">
-        <v>281.44741666666602</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2324" spans="1:3" x14ac:dyDescent="0.25">
@@ -25707,7 +25707,7 @@
         <v>42909</v>
       </c>
       <c r="C2324">
-        <v>314.496499999999</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2325" spans="1:3" x14ac:dyDescent="0.25">
@@ -25715,7 +25715,7 @@
         <v>42910</v>
       </c>
       <c r="C2325">
-        <v>348.33833333333303</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2326" spans="1:3" x14ac:dyDescent="0.25">
@@ -25723,7 +25723,7 @@
         <v>42911</v>
       </c>
       <c r="C2326">
-        <v>328.60149999999999</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2327" spans="1:3" x14ac:dyDescent="0.25">
@@ -25731,7 +25731,7 @@
         <v>42912</v>
       </c>
       <c r="C2327">
-        <v>299.17725000000002</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2328" spans="1:3" x14ac:dyDescent="0.25">
@@ -25739,7 +25739,7 @@
         <v>42913</v>
       </c>
       <c r="C2328">
-        <v>293.41391666666601</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2329" spans="1:3" x14ac:dyDescent="0.25">
@@ -25747,7 +25747,7 @@
         <v>42914</v>
       </c>
       <c r="C2329">
-        <v>289.54258333333303</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2330" spans="1:3" x14ac:dyDescent="0.25">
@@ -25755,7 +25755,7 @@
         <v>42915</v>
       </c>
       <c r="C2330">
-        <v>295.53758333333298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2331" spans="1:3" x14ac:dyDescent="0.25">
@@ -25763,7 +25763,7 @@
         <v>42916</v>
       </c>
       <c r="C2331">
-        <v>308.88916666666597</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2332" spans="1:3" x14ac:dyDescent="0.25">
@@ -25771,7 +25771,7 @@
         <v>42917</v>
       </c>
       <c r="C2332">
-        <v>371.28666666666601</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2333" spans="1:3" x14ac:dyDescent="0.25">
@@ -25779,7 +25779,7 @@
         <v>42918</v>
       </c>
       <c r="C2333">
-        <v>313.356333333333</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2334" spans="1:3" x14ac:dyDescent="0.25">
@@ -25787,7 +25787,7 @@
         <v>42919</v>
       </c>
       <c r="C2334">
-        <v>280.36260714285697</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2335" spans="1:3" x14ac:dyDescent="0.25">
@@ -25795,7 +25795,7 @@
         <v>42920</v>
       </c>
       <c r="C2335">
-        <v>285.12627380952301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2336" spans="1:3" x14ac:dyDescent="0.25">
@@ -25803,7 +25803,7 @@
         <v>42921</v>
       </c>
       <c r="C2336">
-        <v>285.68544047619002</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2337" spans="1:3" x14ac:dyDescent="0.25">
@@ -25811,7 +25811,7 @@
         <v>42922</v>
       </c>
       <c r="C2337">
-        <v>287.02544047619</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2338" spans="1:3" x14ac:dyDescent="0.25">
@@ -25819,7 +25819,7 @@
         <v>42923</v>
       </c>
       <c r="C2338">
-        <v>311.09583333333302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2339" spans="1:3" x14ac:dyDescent="0.25">
@@ -25827,7 +25827,7 @@
         <v>42924</v>
       </c>
       <c r="C2339">
-        <v>373.859166666666</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2340" spans="1:3" x14ac:dyDescent="0.25">
@@ -25835,7 +25835,7 @@
         <v>42925</v>
       </c>
       <c r="C2340">
-        <v>321.63916666666597</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2341" spans="1:3" x14ac:dyDescent="0.25">
@@ -25843,7 +25843,7 @@
         <v>42926</v>
       </c>
       <c r="C2341">
-        <v>283.717107142857</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2342" spans="1:3" x14ac:dyDescent="0.25">
@@ -25851,7 +25851,7 @@
         <v>42927</v>
       </c>
       <c r="C2342">
-        <v>283.55544047618997</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2343" spans="1:3" x14ac:dyDescent="0.25">
@@ -25859,7 +25859,7 @@
         <v>42928</v>
       </c>
       <c r="C2343">
-        <v>282.779916666666</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2344" spans="1:3" x14ac:dyDescent="0.25">
@@ -25867,7 +25867,7 @@
         <v>42929</v>
       </c>
       <c r="C2344">
-        <v>283.94724999999897</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2345" spans="1:3" x14ac:dyDescent="0.25">
@@ -25875,7 +25875,7 @@
         <v>42930</v>
       </c>
       <c r="C2345">
-        <v>305.61250000000001</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2346" spans="1:3" x14ac:dyDescent="0.25">
@@ -25883,7 +25883,7 @@
         <v>42931</v>
       </c>
       <c r="C2346">
-        <v>357.05416666666599</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2347" spans="1:3" x14ac:dyDescent="0.25">
@@ -25891,7 +25891,7 @@
         <v>42932</v>
       </c>
       <c r="C2347">
-        <v>315.74250000000001</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2348" spans="1:3" x14ac:dyDescent="0.25">
@@ -25899,7 +25899,7 @@
         <v>42933</v>
       </c>
       <c r="C2348">
-        <v>281.50708333333301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2349" spans="1:3" x14ac:dyDescent="0.25">
@@ -25907,7 +25907,7 @@
         <v>42934</v>
       </c>
       <c r="C2349">
-        <v>281.481083333333</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2350" spans="1:3" x14ac:dyDescent="0.25">
@@ -25915,7 +25915,7 @@
         <v>42935</v>
       </c>
       <c r="C2350">
-        <v>280.909416666666</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2351" spans="1:3" x14ac:dyDescent="0.25">
@@ -25923,7 +25923,7 @@
         <v>42936</v>
       </c>
       <c r="C2351">
-        <v>276.33941666666601</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2352" spans="1:3" x14ac:dyDescent="0.25">
@@ -25931,7 +25931,7 @@
         <v>42937</v>
       </c>
       <c r="C2352">
-        <v>295.42083333333301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2353" spans="1:3" x14ac:dyDescent="0.25">
@@ -25939,7 +25939,7 @@
         <v>42938</v>
       </c>
       <c r="C2353">
-        <v>345.870833333333</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2354" spans="1:3" x14ac:dyDescent="0.25">
@@ -25947,7 +25947,7 @@
         <v>42939</v>
       </c>
       <c r="C2354">
-        <v>327.06150000000002</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2355" spans="1:3" x14ac:dyDescent="0.25">
@@ -25955,7 +25955,7 @@
         <v>42940</v>
       </c>
       <c r="C2355">
-        <v>296.83758333333299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2356" spans="1:3" x14ac:dyDescent="0.25">
@@ -25963,7 +25963,7 @@
         <v>42941</v>
       </c>
       <c r="C2356">
-        <v>297.64024999999998</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2357" spans="1:3" x14ac:dyDescent="0.25">
@@ -25971,7 +25971,7 @@
         <v>42942</v>
       </c>
       <c r="C2357">
-        <v>294.14058333333298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2358" spans="1:3" x14ac:dyDescent="0.25">
@@ -25979,7 +25979,7 @@
         <v>42943</v>
       </c>
       <c r="C2358">
-        <v>298.67558333333301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2359" spans="1:3" x14ac:dyDescent="0.25">
@@ -25987,7 +25987,7 @@
         <v>42944</v>
       </c>
       <c r="C2359">
-        <v>309.919166666666</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2360" spans="1:3" x14ac:dyDescent="0.25">
@@ -25995,7 +25995,7 @@
         <v>42945</v>
       </c>
       <c r="C2360">
-        <v>344.34666666666601</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2361" spans="1:3" x14ac:dyDescent="0.25">
@@ -26003,7 +26003,7 @@
         <v>42946</v>
       </c>
       <c r="C2361">
-        <v>316.12983333333301</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2362" spans="1:3" x14ac:dyDescent="0.25">
@@ -26011,7 +26011,7 @@
         <v>42947</v>
       </c>
       <c r="C2362">
-        <v>297.49675000000002</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2363" spans="1:3" x14ac:dyDescent="0.25">
@@ -26019,7 +26019,7 @@
         <v>42948</v>
       </c>
       <c r="C2363">
-        <v>279.01635714285698</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2364" spans="1:3" x14ac:dyDescent="0.25">
@@ -26027,7 +26027,7 @@
         <v>42949</v>
       </c>
       <c r="C2364">
-        <v>279.02635714285702</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2365" spans="1:3" x14ac:dyDescent="0.25">
@@ -26035,7 +26035,7 @@
         <v>42950</v>
       </c>
       <c r="C2365">
-        <v>284.29094047618997</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2366" spans="1:3" x14ac:dyDescent="0.25">
@@ -26043,7 +26043,7 @@
         <v>42951</v>
       </c>
       <c r="C2366">
-        <v>316.04333333333301</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2367" spans="1:3" x14ac:dyDescent="0.25">
@@ -26051,7 +26051,7 @@
         <v>42952</v>
       </c>
       <c r="C2367">
-        <v>374.28416666666601</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2368" spans="1:3" x14ac:dyDescent="0.25">
@@ -26059,7 +26059,7 @@
         <v>42953</v>
       </c>
       <c r="C2368">
-        <v>320.83583333333303</v>
+        <v>320</v>
       </c>
     </row>
     <row r="2369" spans="1:3" x14ac:dyDescent="0.25">
@@ -26067,7 +26067,7 @@
         <v>42954</v>
       </c>
       <c r="C2369">
-        <v>284.57210714285702</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2370" spans="1:3" x14ac:dyDescent="0.25">
@@ -26075,7 +26075,7 @@
         <v>42955</v>
       </c>
       <c r="C2370">
-        <v>284.16877380952297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2371" spans="1:3" x14ac:dyDescent="0.25">
@@ -26083,7 +26083,7 @@
         <v>42956</v>
       </c>
       <c r="C2371">
-        <v>282.10544047618998</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2372" spans="1:3" x14ac:dyDescent="0.25">
@@ -26091,7 +26091,7 @@
         <v>42957</v>
       </c>
       <c r="C2372">
-        <v>285.50710714285702</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2373" spans="1:3" x14ac:dyDescent="0.25">
@@ -26099,7 +26099,7 @@
         <v>42958</v>
       </c>
       <c r="C2373">
-        <v>312.00749999999999</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2374" spans="1:3" x14ac:dyDescent="0.25">
@@ -26107,7 +26107,7 @@
         <v>42959</v>
       </c>
       <c r="C2374">
-        <v>368.41416666666601</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2375" spans="1:3" x14ac:dyDescent="0.25">
@@ -26115,7 +26115,7 @@
         <v>42960</v>
       </c>
       <c r="C2375">
-        <v>321.51749999999998</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2376" spans="1:3" x14ac:dyDescent="0.25">
@@ -26123,7 +26123,7 @@
         <v>42961</v>
       </c>
       <c r="C2376">
-        <v>284.86474999999899</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2377" spans="1:3" x14ac:dyDescent="0.25">
@@ -26131,7 +26131,7 @@
         <v>42962</v>
       </c>
       <c r="C2377">
-        <v>283.87641666666599</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2378" spans="1:3" x14ac:dyDescent="0.25">
@@ -26139,7 +26139,7 @@
         <v>42963</v>
       </c>
       <c r="C2378">
-        <v>279.97874999999999</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2379" spans="1:3" x14ac:dyDescent="0.25">
@@ -26147,7 +26147,7 @@
         <v>42964</v>
       </c>
       <c r="C2379">
-        <v>279.92541666666602</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2380" spans="1:3" x14ac:dyDescent="0.25">
@@ -26155,7 +26155,7 @@
         <v>42965</v>
       </c>
       <c r="C2380">
-        <v>303.0865</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2381" spans="1:3" x14ac:dyDescent="0.25">
@@ -26163,7 +26163,7 @@
         <v>42966</v>
       </c>
       <c r="C2381">
-        <v>339.82749999999999</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2382" spans="1:3" x14ac:dyDescent="0.25">
@@ -26171,7 +26171,7 @@
         <v>42967</v>
       </c>
       <c r="C2382">
-        <v>314.80149999999998</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2383" spans="1:3" x14ac:dyDescent="0.25">
@@ -26179,7 +26179,7 @@
         <v>42968</v>
       </c>
       <c r="C2383">
-        <v>281.52108333333302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2384" spans="1:3" x14ac:dyDescent="0.25">
@@ -26187,7 +26187,7 @@
         <v>42969</v>
       </c>
       <c r="C2384">
-        <v>282.89408333333301</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2385" spans="1:3" x14ac:dyDescent="0.25">
@@ -26195,7 +26195,7 @@
         <v>42970</v>
       </c>
       <c r="C2385">
-        <v>293.74924999999899</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2386" spans="1:3" x14ac:dyDescent="0.25">
@@ -26203,7 +26203,7 @@
         <v>42971</v>
       </c>
       <c r="C2386">
-        <v>295.98591666666601</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2387" spans="1:3" x14ac:dyDescent="0.25">
@@ -26211,7 +26211,7 @@
         <v>42972</v>
       </c>
       <c r="C2387">
-        <v>316.67716666666598</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2388" spans="1:3" x14ac:dyDescent="0.25">
@@ -26219,7 +26219,7 @@
         <v>42973</v>
       </c>
       <c r="C2388">
-        <v>347.54766666666598</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2389" spans="1:3" x14ac:dyDescent="0.25">
@@ -26227,7 +26227,7 @@
         <v>42974</v>
       </c>
       <c r="C2389">
-        <v>322.86483333333302</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2390" spans="1:3" x14ac:dyDescent="0.25">
@@ -26235,7 +26235,7 @@
         <v>42975</v>
       </c>
       <c r="C2390">
-        <v>299.92925000000002</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2391" spans="1:3" x14ac:dyDescent="0.25">
@@ -26243,7 +26243,7 @@
         <v>42976</v>
       </c>
       <c r="C2391">
-        <v>294.73841666666601</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2392" spans="1:3" x14ac:dyDescent="0.25">
@@ -26251,7 +26251,7 @@
         <v>42977</v>
       </c>
       <c r="C2392">
-        <v>292.262583333333</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2393" spans="1:3" x14ac:dyDescent="0.25">
@@ -26259,7 +26259,7 @@
         <v>42978</v>
       </c>
       <c r="C2393">
-        <v>298.567583333333</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2394" spans="1:3" x14ac:dyDescent="0.25">
@@ -26267,7 +26267,7 @@
         <v>42979</v>
       </c>
       <c r="C2394">
-        <v>307.76433333333301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2395" spans="1:3" x14ac:dyDescent="0.25">
@@ -26275,7 +26275,7 @@
         <v>42980</v>
       </c>
       <c r="C2395">
-        <v>371.07666666666597</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2396" spans="1:3" x14ac:dyDescent="0.25">
@@ -26283,7 +26283,7 @@
         <v>42981</v>
       </c>
       <c r="C2396">
-        <v>314.62633333333298</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2397" spans="1:3" x14ac:dyDescent="0.25">
@@ -26291,7 +26291,7 @@
         <v>42982</v>
       </c>
       <c r="C2397">
-        <v>286.65094047618999</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2398" spans="1:3" x14ac:dyDescent="0.25">
@@ -26299,7 +26299,7 @@
         <v>42983</v>
       </c>
       <c r="C2398">
-        <v>286.46177380952298</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2399" spans="1:3" x14ac:dyDescent="0.25">
@@ -26307,7 +26307,7 @@
         <v>42984</v>
       </c>
       <c r="C2399">
-        <v>283.46177380952298</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2400" spans="1:3" x14ac:dyDescent="0.25">
@@ -26315,7 +26315,7 @@
         <v>42985</v>
       </c>
       <c r="C2400">
-        <v>286.066773809523</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2401" spans="1:3" x14ac:dyDescent="0.25">
@@ -26323,7 +26323,7 @@
         <v>42986</v>
       </c>
       <c r="C2401">
-        <v>310.88383333333297</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2402" spans="1:3" x14ac:dyDescent="0.25">
@@ -26331,7 +26331,7 @@
         <v>42987</v>
       </c>
       <c r="C2402">
-        <v>368.78916666666601</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2403" spans="1:3" x14ac:dyDescent="0.25">
@@ -26339,7 +26339,7 @@
         <v>42988</v>
       </c>
       <c r="C2403">
-        <v>319.32583333333298</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2404" spans="1:3" x14ac:dyDescent="0.25">
@@ -26347,7 +26347,7 @@
         <v>42989</v>
       </c>
       <c r="C2404">
-        <v>285.44344047619001</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2405" spans="1:3" x14ac:dyDescent="0.25">
@@ -26355,7 +26355,7 @@
         <v>42990</v>
       </c>
       <c r="C2405">
-        <v>285.02625</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2406" spans="1:3" x14ac:dyDescent="0.25">
@@ -26363,7 +26363,7 @@
         <v>42991</v>
       </c>
       <c r="C2406">
-        <v>282.99191666666599</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2407" spans="1:3" x14ac:dyDescent="0.25">
@@ -26371,7 +26371,7 @@
         <v>42992</v>
       </c>
       <c r="C2407">
-        <v>282.36774999999898</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2408" spans="1:3" x14ac:dyDescent="0.25">
@@ -26379,7 +26379,7 @@
         <v>42993</v>
       </c>
       <c r="C2408">
-        <v>306.90449999999998</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2409" spans="1:3" x14ac:dyDescent="0.25">
@@ -26387,7 +26387,7 @@
         <v>42994</v>
       </c>
       <c r="C2409">
-        <v>345.90416666666601</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2410" spans="1:3" x14ac:dyDescent="0.25">
@@ -26395,7 +26395,7 @@
         <v>42995</v>
       </c>
       <c r="C2410">
-        <v>315.34249999999997</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2411" spans="1:3" x14ac:dyDescent="0.25">
@@ -26403,7 +26403,7 @@
         <v>42996</v>
       </c>
       <c r="C2411">
-        <v>283.00441666666597</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2412" spans="1:3" x14ac:dyDescent="0.25">
@@ -26411,7 +26411,7 @@
         <v>42997</v>
       </c>
       <c r="C2412">
-        <v>284.03774999999899</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2413" spans="1:3" x14ac:dyDescent="0.25">
@@ -26419,7 +26419,7 @@
         <v>42998</v>
       </c>
       <c r="C2413">
-        <v>277.83774999999901</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2414" spans="1:3" x14ac:dyDescent="0.25">
@@ -26427,7 +26427,7 @@
         <v>42999</v>
       </c>
       <c r="C2414">
-        <v>275.92441666666599</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2415" spans="1:3" x14ac:dyDescent="0.25">
@@ -26435,7 +26435,7 @@
         <v>43000</v>
       </c>
       <c r="C2415">
-        <v>305.65783333333297</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2416" spans="1:3" x14ac:dyDescent="0.25">
@@ -26443,7 +26443,7 @@
         <v>43001</v>
       </c>
       <c r="C2416">
-        <v>349.370833333333</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2417" spans="1:3" x14ac:dyDescent="0.25">
@@ -26451,7 +26451,7 @@
         <v>43002</v>
       </c>
       <c r="C2417">
-        <v>325.22983333333298</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2418" spans="1:3" x14ac:dyDescent="0.25">
@@ -26459,7 +26459,7 @@
         <v>43003</v>
       </c>
       <c r="C2418">
-        <v>302.09025000000003</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2419" spans="1:3" x14ac:dyDescent="0.25">
@@ -26467,7 +26467,7 @@
         <v>43004</v>
       </c>
       <c r="C2419">
-        <v>298.32891666666598</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2420" spans="1:3" x14ac:dyDescent="0.25">
@@ -26475,7 +26475,7 @@
         <v>43005</v>
       </c>
       <c r="C2420">
-        <v>293.23058333333302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2421" spans="1:3" x14ac:dyDescent="0.25">
@@ -26483,7 +26483,7 @@
         <v>43006</v>
       </c>
       <c r="C2421">
-        <v>297.34758333333298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2422" spans="1:3" x14ac:dyDescent="0.25">
@@ -26491,7 +26491,7 @@
         <v>43007</v>
       </c>
       <c r="C2422">
-        <v>310.52916666666601</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2423" spans="1:3" x14ac:dyDescent="0.25">
@@ -26499,7 +26499,7 @@
         <v>43008</v>
       </c>
       <c r="C2423">
-        <v>343.29</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2424" spans="1:3" x14ac:dyDescent="0.25">
@@ -26507,7 +26507,7 @@
         <v>43009</v>
       </c>
       <c r="C2424">
-        <v>313.09800000000001</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2425" spans="1:3" x14ac:dyDescent="0.25">
@@ -26515,7 +26515,7 @@
         <v>43010</v>
       </c>
       <c r="C2425">
-        <v>279.76435714285702</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2426" spans="1:3" x14ac:dyDescent="0.25">
@@ -26523,7 +26523,7 @@
         <v>43011</v>
       </c>
       <c r="C2426">
-        <v>280.98560714285702</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2427" spans="1:3" x14ac:dyDescent="0.25">
@@ -26531,7 +26531,7 @@
         <v>43012</v>
       </c>
       <c r="C2427">
-        <v>286.09594047618998</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2428" spans="1:3" x14ac:dyDescent="0.25">
@@ -26539,7 +26539,7 @@
         <v>43013</v>
       </c>
       <c r="C2428">
-        <v>290.99510714285702</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2429" spans="1:3" x14ac:dyDescent="0.25">
@@ -26547,7 +26547,7 @@
         <v>43014</v>
       </c>
       <c r="C2429">
-        <v>313.75716666666602</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2430" spans="1:3" x14ac:dyDescent="0.25">
@@ -26555,7 +26555,7 @@
         <v>43015</v>
       </c>
       <c r="C2430">
-        <v>375.56916666666598</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2431" spans="1:3" x14ac:dyDescent="0.25">
@@ -26563,7 +26563,7 @@
         <v>43016</v>
       </c>
       <c r="C2431">
-        <v>321.674166666666</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2432" spans="1:3" x14ac:dyDescent="0.25">
@@ -26571,7 +26571,7 @@
         <v>43017</v>
       </c>
       <c r="C2432">
-        <v>284.63677380952299</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2433" spans="1:3" x14ac:dyDescent="0.25">
@@ -26579,7 +26579,7 @@
         <v>43018</v>
       </c>
       <c r="C2433">
-        <v>284.90177380952298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2434" spans="1:3" x14ac:dyDescent="0.25">
@@ -26587,7 +26587,7 @@
         <v>43019</v>
       </c>
       <c r="C2434">
-        <v>284.05844047619001</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2435" spans="1:3" x14ac:dyDescent="0.25">
@@ -26595,7 +26595,7 @@
         <v>43020</v>
       </c>
       <c r="C2435">
-        <v>286.44458333333301</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2436" spans="1:3" x14ac:dyDescent="0.25">
@@ -26603,7 +26603,7 @@
         <v>43021</v>
       </c>
       <c r="C2436">
-        <v>309.20616666666598</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2437" spans="1:3" x14ac:dyDescent="0.25">
@@ -26611,7 +26611,7 @@
         <v>43022</v>
       </c>
       <c r="C2437">
-        <v>357.854166666666</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2438" spans="1:3" x14ac:dyDescent="0.25">
@@ -26619,7 +26619,7 @@
         <v>43023</v>
       </c>
       <c r="C2438">
-        <v>318.02749999999997</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2439" spans="1:3" x14ac:dyDescent="0.25">
@@ -26627,7 +26627,7 @@
         <v>43024</v>
       </c>
       <c r="C2439">
-        <v>283.14674999999897</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2440" spans="1:3" x14ac:dyDescent="0.25">
@@ -26635,7 +26635,7 @@
         <v>43025</v>
       </c>
       <c r="C2440">
-        <v>282.93341666666601</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2441" spans="1:3" x14ac:dyDescent="0.25">
@@ -26643,7 +26643,7 @@
         <v>43026</v>
       </c>
       <c r="C2441">
-        <v>281.06608333333298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2442" spans="1:3" x14ac:dyDescent="0.25">
@@ -26651,7 +26651,7 @@
         <v>43027</v>
       </c>
       <c r="C2442">
-        <v>281.90441666666601</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2443" spans="1:3" x14ac:dyDescent="0.25">
@@ -26659,7 +26659,7 @@
         <v>43028</v>
       </c>
       <c r="C2443">
-        <v>300.21316666666598</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2444" spans="1:3" x14ac:dyDescent="0.25">
@@ -26667,7 +26667,7 @@
         <v>43029</v>
       </c>
       <c r="C2444">
-        <v>337.51083333333298</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2445" spans="1:3" x14ac:dyDescent="0.25">
@@ -26675,7 +26675,7 @@
         <v>43030</v>
       </c>
       <c r="C2445">
-        <v>316.72899999999998</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2446" spans="1:3" x14ac:dyDescent="0.25">
@@ -26683,7 +26683,7 @@
         <v>43031</v>
       </c>
       <c r="C2446">
-        <v>300.33341666666598</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2447" spans="1:3" x14ac:dyDescent="0.25">
@@ -26691,7 +26691,7 @@
         <v>43032</v>
       </c>
       <c r="C2447">
-        <v>295.36591666666601</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2448" spans="1:3" x14ac:dyDescent="0.25">
@@ -26699,7 +26699,7 @@
         <v>43033</v>
       </c>
       <c r="C2448">
-        <v>295.83524999999997</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2449" spans="1:3" x14ac:dyDescent="0.25">
@@ -26707,7 +26707,7 @@
         <v>43034</v>
       </c>
       <c r="C2449">
-        <v>300.66891666666601</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2450" spans="1:3" x14ac:dyDescent="0.25">
@@ -26715,7 +26715,7 @@
         <v>43035</v>
       </c>
       <c r="C2450">
-        <v>313.62249999999898</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2451" spans="1:3" x14ac:dyDescent="0.25">
@@ -26723,7 +26723,7 @@
         <v>43036</v>
       </c>
       <c r="C2451">
-        <v>345.390999999999</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2452" spans="1:3" x14ac:dyDescent="0.25">
@@ -26731,7 +26731,7 @@
         <v>43037</v>
       </c>
       <c r="C2452">
-        <v>316.84233333333299</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2453" spans="1:3" x14ac:dyDescent="0.25">
@@ -26739,7 +26739,7 @@
         <v>43038</v>
       </c>
       <c r="C2453">
-        <v>299.16258333333298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2454" spans="1:3" x14ac:dyDescent="0.25">
@@ -26747,7 +26747,7 @@
         <v>43039</v>
       </c>
       <c r="C2454">
-        <v>294.40174999999999</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2455" spans="1:3" x14ac:dyDescent="0.25">
@@ -26755,7 +26755,7 @@
         <v>43040</v>
       </c>
       <c r="C2455">
-        <v>279.598023809523</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2456" spans="1:3" x14ac:dyDescent="0.25">
@@ -26763,7 +26763,7 @@
         <v>43041</v>
       </c>
       <c r="C2456">
-        <v>283.163023809523</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2457" spans="1:3" x14ac:dyDescent="0.25">
@@ -26771,7 +26771,7 @@
         <v>43042</v>
       </c>
       <c r="C2457">
-        <v>311.94966666666602</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2458" spans="1:3" x14ac:dyDescent="0.25">
@@ -26779,7 +26779,7 @@
         <v>43043</v>
       </c>
       <c r="C2458">
-        <v>375.97</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2459" spans="1:3" x14ac:dyDescent="0.25">
@@ -26787,7 +26787,7 @@
         <v>43044</v>
       </c>
       <c r="C2459">
-        <v>323.75916666666598</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2460" spans="1:3" x14ac:dyDescent="0.25">
@@ -26795,7 +26795,7 @@
         <v>43045</v>
       </c>
       <c r="C2460">
-        <v>285.51710714285701</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2461" spans="1:3" x14ac:dyDescent="0.25">
@@ -26803,7 +26803,7 @@
         <v>43046</v>
       </c>
       <c r="C2461">
-        <v>284.42877380952302</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2462" spans="1:3" x14ac:dyDescent="0.25">
@@ -26811,7 +26811,7 @@
         <v>43047</v>
       </c>
       <c r="C2462">
-        <v>283.96877380952299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2463" spans="1:3" x14ac:dyDescent="0.25">
@@ -26819,7 +26819,7 @@
         <v>43048</v>
       </c>
       <c r="C2463">
-        <v>286.45044047619001</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2464" spans="1:3" x14ac:dyDescent="0.25">
@@ -26827,7 +26827,7 @@
         <v>43049</v>
       </c>
       <c r="C2464">
-        <v>314.39583333333297</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2465" spans="1:3" x14ac:dyDescent="0.25">
@@ -26835,7 +26835,7 @@
         <v>43050</v>
       </c>
       <c r="C2465">
-        <v>373.7475</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2466" spans="1:3" x14ac:dyDescent="0.25">
@@ -26843,7 +26843,7 @@
         <v>43051</v>
       </c>
       <c r="C2466">
-        <v>323.92950000000002</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2467" spans="1:3" x14ac:dyDescent="0.25">
@@ -26851,7 +26851,7 @@
         <v>43052</v>
       </c>
       <c r="C2467">
-        <v>287.62225000000001</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2468" spans="1:3" x14ac:dyDescent="0.25">
@@ -26859,7 +26859,7 @@
         <v>43053</v>
       </c>
       <c r="C2468">
-        <v>285.71474999999901</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2469" spans="1:3" x14ac:dyDescent="0.25">
@@ -26867,7 +26867,7 @@
         <v>43054</v>
       </c>
       <c r="C2469">
-        <v>283.73308333333301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2470" spans="1:3" x14ac:dyDescent="0.25">
@@ -26875,7 +26875,7 @@
         <v>43055</v>
       </c>
       <c r="C2470">
-        <v>281.78041666666599</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2471" spans="1:3" x14ac:dyDescent="0.25">
@@ -26883,7 +26883,7 @@
         <v>43056</v>
       </c>
       <c r="C2471">
-        <v>305.0265</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2472" spans="1:3" x14ac:dyDescent="0.25">
@@ -26891,7 +26891,7 @@
         <v>43057</v>
       </c>
       <c r="C2472">
-        <v>343.86416666666599</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2473" spans="1:3" x14ac:dyDescent="0.25">
@@ -26899,7 +26899,7 @@
         <v>43058</v>
       </c>
       <c r="C2473">
-        <v>319.68316666666601</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2474" spans="1:3" x14ac:dyDescent="0.25">
@@ -26907,7 +26907,7 @@
         <v>43059</v>
       </c>
       <c r="C2474">
-        <v>283.39108333333297</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2475" spans="1:3" x14ac:dyDescent="0.25">
@@ -26915,7 +26915,7 @@
         <v>43060</v>
       </c>
       <c r="C2475">
-        <v>281.08608333333302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2476" spans="1:3" x14ac:dyDescent="0.25">
@@ -26923,7 +26923,7 @@
         <v>43061</v>
       </c>
       <c r="C2476">
-        <v>281.90074999999899</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2477" spans="1:3" x14ac:dyDescent="0.25">
@@ -26931,7 +26931,7 @@
         <v>43062</v>
       </c>
       <c r="C2477">
-        <v>299.315916666666</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2478" spans="1:3" x14ac:dyDescent="0.25">
@@ -26939,7 +26939,7 @@
         <v>43063</v>
       </c>
       <c r="C2478">
-        <v>315.27816666666598</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2479" spans="1:3" x14ac:dyDescent="0.25">
@@ -26947,7 +26947,7 @@
         <v>43064</v>
       </c>
       <c r="C2479">
-        <v>348.04433333333299</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2480" spans="1:3" x14ac:dyDescent="0.25">
@@ -26955,7 +26955,7 @@
         <v>43065</v>
       </c>
       <c r="C2480">
-        <v>329.950666666666</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2481" spans="1:3" x14ac:dyDescent="0.25">
@@ -26963,7 +26963,7 @@
         <v>43066</v>
       </c>
       <c r="C2481">
-        <v>301.871178571428</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2482" spans="1:3" x14ac:dyDescent="0.25">
@@ -26971,7 +26971,7 @@
         <v>43067</v>
       </c>
       <c r="C2482">
-        <v>296.37734523809502</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2483" spans="1:3" x14ac:dyDescent="0.25">
@@ -26979,7 +26979,7 @@
         <v>43068</v>
       </c>
       <c r="C2483">
-        <v>292.17401190476102</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2484" spans="1:3" x14ac:dyDescent="0.25">
@@ -26987,7 +26987,7 @@
         <v>43069</v>
       </c>
       <c r="C2484">
-        <v>299.26758333333299</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2485" spans="1:3" x14ac:dyDescent="0.25">
@@ -26995,7 +26995,7 @@
         <v>43070</v>
       </c>
       <c r="C2485">
-        <v>311.029666666666</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2486" spans="1:3" x14ac:dyDescent="0.25">
@@ -27003,7 +27003,7 @@
         <v>43071</v>
       </c>
       <c r="C2486">
-        <v>374.78</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2487" spans="1:3" x14ac:dyDescent="0.25">
@@ -27011,7 +27011,7 @@
         <v>43072</v>
       </c>
       <c r="C2487">
-        <v>315.43466666666598</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2488" spans="1:3" x14ac:dyDescent="0.25">
@@ -27019,7 +27019,7 @@
         <v>43073</v>
       </c>
       <c r="C2488">
-        <v>287.166607142857</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2489" spans="1:3" x14ac:dyDescent="0.25">
@@ -27027,7 +27027,7 @@
         <v>43074</v>
       </c>
       <c r="C2489">
-        <v>288.48577380952298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2490" spans="1:3" x14ac:dyDescent="0.25">
@@ -27035,7 +27035,7 @@
         <v>43075</v>
       </c>
       <c r="C2490">
-        <v>285.57577380952301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2491" spans="1:3" x14ac:dyDescent="0.25">
@@ -27043,7 +27043,7 @@
         <v>43076</v>
       </c>
       <c r="C2491">
-        <v>288.08877380952299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2492" spans="1:3" x14ac:dyDescent="0.25">
@@ -27051,7 +27051,7 @@
         <v>43077</v>
       </c>
       <c r="C2492">
-        <v>314.83416666666602</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2493" spans="1:3" x14ac:dyDescent="0.25">
@@ -27059,7 +27059,7 @@
         <v>43078</v>
       </c>
       <c r="C2493">
-        <v>372.11250000000001</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2494" spans="1:3" x14ac:dyDescent="0.25">
@@ -27067,7 +27067,7 @@
         <v>43079</v>
       </c>
       <c r="C2494">
-        <v>322.02449999999999</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2495" spans="1:3" x14ac:dyDescent="0.25">
@@ -27075,7 +27075,7 @@
         <v>43080</v>
       </c>
       <c r="C2495">
-        <v>286.40377380952299</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2496" spans="1:3" x14ac:dyDescent="0.25">
@@ -27083,7 +27083,7 @@
         <v>43081</v>
       </c>
       <c r="C2496">
-        <v>287.30324999999999</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2497" spans="1:3" x14ac:dyDescent="0.25">
@@ -27091,7 +27091,7 @@
         <v>43082</v>
       </c>
       <c r="C2497">
-        <v>285.39891666666603</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2498" spans="1:3" x14ac:dyDescent="0.25">
@@ -27099,7 +27099,7 @@
         <v>43083</v>
       </c>
       <c r="C2498">
-        <v>285.419749999999</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2499" spans="1:3" x14ac:dyDescent="0.25">
@@ -27107,7 +27107,7 @@
         <v>43084</v>
       </c>
       <c r="C2499">
-        <v>309.91983333333297</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2500" spans="1:3" x14ac:dyDescent="0.25">
@@ -27115,7 +27115,7 @@
         <v>43085</v>
       </c>
       <c r="C2500">
-        <v>345.25749999999999</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2501" spans="1:3" x14ac:dyDescent="0.25">
@@ -27123,7 +27123,7 @@
         <v>43086</v>
       </c>
       <c r="C2501">
-        <v>319.41416666666601</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2502" spans="1:3" x14ac:dyDescent="0.25">
@@ -27131,7 +27131,7 @@
         <v>43087</v>
       </c>
       <c r="C2502">
-        <v>285.59108333333302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2503" spans="1:3" x14ac:dyDescent="0.25">
@@ -27139,7 +27139,7 @@
         <v>43088</v>
       </c>
       <c r="C2503">
-        <v>285.42274999999898</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2504" spans="1:3" x14ac:dyDescent="0.25">
@@ -27147,7 +27147,7 @@
         <v>43089</v>
       </c>
       <c r="C2504">
-        <v>280.54274999999899</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2505" spans="1:3" x14ac:dyDescent="0.25">
@@ -27155,7 +27155,7 @@
         <v>43090</v>
       </c>
       <c r="C2505">
-        <v>278.88441666666603</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2506" spans="1:3" x14ac:dyDescent="0.25">
@@ -27163,7 +27163,7 @@
         <v>43091</v>
       </c>
       <c r="C2506">
-        <v>308.69116666666599</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2507" spans="1:3" x14ac:dyDescent="0.25">
@@ -27171,7 +27171,7 @@
         <v>43092</v>
       </c>
       <c r="C2507">
-        <v>349.48750000000001</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2508" spans="1:3" x14ac:dyDescent="0.25">
@@ -27179,7 +27179,7 @@
         <v>43093</v>
       </c>
       <c r="C2508">
-        <v>330.12066666666601</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2509" spans="1:3" x14ac:dyDescent="0.25">
@@ -27187,7 +27187,7 @@
         <v>43094</v>
       </c>
       <c r="C2509">
-        <v>303.89774999999997</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2510" spans="1:3" x14ac:dyDescent="0.25">
@@ -27195,7 +27195,7 @@
         <v>43095</v>
       </c>
       <c r="C2510">
-        <v>301.733916666666</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2511" spans="1:3" x14ac:dyDescent="0.25">
@@ -27203,7 +27203,7 @@
         <v>43096</v>
       </c>
       <c r="C2511">
-        <v>297.51201190476098</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2512" spans="1:3" x14ac:dyDescent="0.25">
@@ -27211,7 +27211,7 @@
         <v>43097</v>
       </c>
       <c r="C2512">
-        <v>300.77508333333299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2513" spans="1:3" x14ac:dyDescent="0.25">
@@ -27219,7 +27219,7 @@
         <v>43098</v>
       </c>
       <c r="C2513">
-        <v>314.12666666666598</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2514" spans="1:3" x14ac:dyDescent="0.25">
@@ -27227,7 +27227,7 @@
         <v>43099</v>
       </c>
       <c r="C2514">
-        <v>342.40666666666601</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2515" spans="1:3" x14ac:dyDescent="0.25">
@@ -27235,7 +27235,7 @@
         <v>43100</v>
       </c>
       <c r="C2515">
-        <v>320.99709523809503</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>